<commit_message>
Fix for charts/images offset from a hidden cell.
Fix for worksheet objects (charts and images) that are inserted
with an offset that starts in a hidden cell.
</commit_message>
<xml_diff>
--- a/test/regression/xlsx_files/image45.xlsx
+++ b/test/regression/xlsx_files/image45.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -67,8 +67,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>

</xml_diff>